<commit_message>
upd, minor corrections, annotations
</commit_message>
<xml_diff>
--- a/szondi/WITprose/ff-codes_2.xlsx
+++ b/szondi/WITprose/ff-codes_2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="221" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="221" uniqueCount="77">
   <si>
     <t>Farbe</t>
   </si>
@@ -225,22 +225,25 @@
     <t>später striemenlos im stall</t>
   </si>
   <si>
-    <t>28.01.25 19:03</t>
+    <t>29.01.25 05:59</t>
   </si>
   <si>
     <t>22.01.25 11:30:25</t>
   </si>
   <si>
-    <t>strieme: engl. weal &gt; wheelless &gt; radlos &gt; ratlos</t>
-  </si>
-  <si>
-    <t>und falls wendig, fast wie wasser, über vers und hügel, maß und tal, dass keiner einen riegel schöbe vor den quell, eine regel, strenge ruten</t>
-  </si>
-  <si>
-    <t>22.01.25 11:30</t>
+    <t>strieme: engl. weal &gt; wheelless &gt; radlos &gt; ratlos: ratlos im Stall (dt. Idiom?)</t>
+  </si>
+  <si>
+    <t>wendig</t>
+  </si>
+  <si>
+    <t>29.01.25 06:14</t>
   </si>
   <si>
     <t>22.01.25 11:30:52</t>
+  </si>
+  <si>
+    <t>engl.: astute &gt; Stute</t>
   </si>
 </sst>
 </file>
@@ -1494,13 +1497,13 @@
         <v>25</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="O18" s="4">
-        <v>141</v>
+        <v>6</v>
       </c>
       <c r="P18" s="6">
-        <v>1.3218300000000001</v>
+        <v>0.05624824224242992</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>18</v>

</xml_diff>